<commit_message>
finish export json data
</commit_message>
<xml_diff>
--- a/test/cfgxls/测试.xlsx
+++ b/test/cfgxls/测试.xlsx
@@ -1,88 +1,225 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="29868" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reward</t>
+  </si>
+  <si>
+    <t>注释</t>
+  </si>
+  <si>
+    <t>掉落奖励</t>
   </si>
   <si>
     <t>str</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>这是注释</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>reward</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>str</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>掉落奖励</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>填drop表的id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>注释</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,12 +234,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -125,30 +448,316 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -197,7 +806,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,7 +841,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,64 +1044,80 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="14.625" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="1" max="2" width="14.6296296296296" customWidth="1"/>
+    <col min="3" max="3" width="22.3796296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="1" ht="15.6" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="2" ht="15.6" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" ht="15.6" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="4" ht="15.6" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>1001</v>
+      </c>
+      <c r="C5">
+        <v>6001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>1002</v>
+      </c>
+      <c r="C6">
+        <v>6002</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix export string json bug
</commit_message>
<xml_diff>
--- a/test/cfgxls/测试.xlsx
+++ b/test/cfgxls/测试.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\RTM\test\cfgxls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29865" windowHeight="13380"/>
+    <workbookView windowWidth="29868" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +28,10 @@
     <t>掉落奖励</t>
   </si>
   <si>
-    <t>str</t>
+    <t>uint</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
   <si>
     <t>这是注释</t>
@@ -41,16 +39,18 @@
   <si>
     <t>填drop表的id</t>
   </si>
-  <si>
-    <t>uint</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,13 +71,151 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,12 +230,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -120,9 +444,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -133,17 +699,61 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -430,25 +1040,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="2" width="14.625" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="1" max="2" width="14.6296296296296" customWidth="1"/>
+    <col min="3" max="3" width="22.3796296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="1" ht="15.6" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="2" ht="15.6" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,25 +1078,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" ht="15.6" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="4" ht="15.6" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>1001</v>
       </c>
@@ -494,7 +1104,7 @@
         <v>6001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>1002</v>
       </c>
@@ -503,8 +1113,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>